<commit_message>
rename input_keys to input_events, allow disbaling mouse and keyboard separately as well as disable_input
</commit_message>
<xml_diff>
--- a/docs/version_scheduling/0.0.10.xlsx
+++ b/docs/version_scheduling/0.0.10.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mario\Zombono\docs\version_scheduling\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BCCABCAB-A0BC-4452-84C2-E72A16358268}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7579E994-976B-46A0-ABBB-ECB59A197F87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{D1946CF8-FB30-4F75-8FAB-4791887877CB}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="31">
   <si>
     <t>Zombono v0.0.10</t>
   </si>
@@ -45,9 +45,6 @@
     <t>Area</t>
   </si>
   <si>
-    <t>Split qfiles.h - bsp.h, md2.h, sp2.h</t>
-  </si>
-  <si>
     <t>Refactoring</t>
   </si>
   <si>
@@ -57,9 +54,6 @@
     <t>Engineering</t>
   </si>
   <si>
-    <t>Bugfixes</t>
-  </si>
-  <si>
     <t>Yes</t>
   </si>
   <si>
@@ -69,14 +63,62 @@
     <t>Feature</t>
   </si>
   <si>
-    <t>Fix: surface and content flags (Zombono230 MAP format saving those flags)</t>
-  </si>
-  <si>
-    <t>Fix: Jumping from a surface must maintain its relative velocity</t>
-  </si>
-  <si>
-    <t xml:space="preserve">in the ramp on the roof of the mouving platform and the two big one on another map if you move a little bit it start sliding off on it's own, it's not really sliding, but more like jumping
+    <t>Bugfix</t>
+  </si>
+  <si>
+    <t>Split qfiles.h - bsp.h, md2.h, sp2.h, pak.h</t>
+  </si>
+  <si>
+    <t>Fix: no lighting on top of subway buildings, slight gap on one of them</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fix: Jumping from a surface must maintain its relative velocity
 </t>
+  </si>
+  <si>
+    <t>Fix: Warehouse ramps too steep</t>
+  </si>
+  <si>
+    <t>Fix: surface and content flags</t>
+  </si>
+  <si>
+    <t>Fix: Machine gun cannot gain more ammo from packs while out of ammo</t>
+  </si>
+  <si>
+    <t>Fix: Machine gun infinite ammo if held</t>
+  </si>
+  <si>
+    <t>Fix: Re-implement SURF_NODRAW (was never originally implemented)</t>
+  </si>
+  <si>
+    <t>Fix: Missing background and unusual spacing of TimeUI</t>
+  </si>
+  <si>
+    <t>Fix: Unusual spacing of "SELECT TEAM" text</t>
+  </si>
+  <si>
+    <t>Was map issue</t>
+  </si>
+  <si>
+    <t>Fix: Mouse snapped to (0,0) during intro screen</t>
+  </si>
+  <si>
+    <t>Add map and linear speed command to cl_showinfo</t>
+  </si>
+  <si>
+    <t>Add Planfuslicator behaviour (fudge reload time)</t>
+  </si>
+  <si>
+    <t>Fix: Can still move in TeamUI</t>
+  </si>
+  <si>
+    <t>Continue work on z_waves_port, z_tdm_spire, z_waves_yekaterino</t>
+  </si>
+  <si>
+    <t>Content</t>
+  </si>
+  <si>
+    <t>Fix " velocity increasing but not speed" (prediction miss bug when hitting wall at specific angle sometimes)</t>
   </si>
 </sst>
 </file>
@@ -136,7 +178,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -145,6 +187,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -459,18 +502,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A989902-944C-43B3-895E-43AA8F4AB173}">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E22" sqref="E19:E22"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="70.5703125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="102" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19" style="1" customWidth="1"/>
     <col min="3" max="3" width="22" style="1" customWidth="1"/>
-    <col min="4" max="4" width="17.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.85546875" style="1" customWidth="1"/>
     <col min="5" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
@@ -496,26 +539,26 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
-        <v>6</v>
+    <row r="3" spans="1:4" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A3" s="5" t="s">
+        <v>15</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" s="4">
-        <v>45438.063194444447</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>9</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -523,25 +566,139 @@
         <v>14</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="B6" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D9" s="6">
+        <v>45439</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="57" x14ac:dyDescent="0.2">
-      <c r="A8" s="5" t="s">
-        <v>16</v>
+      <c r="B15" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D15" s="4">
+        <v>45438.063194444447</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Remove gl_saturatelighting, adds <60 fps notice text
</commit_message>
<xml_diff>
--- a/docs/version_scheduling/0.0.10.xlsx
+++ b/docs/version_scheduling/0.0.10.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mario\Zombono\docs\version_scheduling\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{144637AE-16BA-4F70-B61D-C7E071832FC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A67E4F1B-9DB9-436D-A693-6CAFB21BFE49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{D1946CF8-FB30-4F75-8FAB-4791887877CB}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="39">
   <si>
     <t>Zombono v0.0.10</t>
   </si>
@@ -136,6 +136,33 @@
   </si>
   <si>
     <t>Fix armour</t>
+  </si>
+  <si>
+    <r>
+      <t>29/05/2024 (</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>REQUIRES POLISHING</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <t>Fix: Game connects to server during intro on Playtest builds</t>
   </si>
 </sst>
 </file>
@@ -519,10 +546,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A989902-944C-43B3-895E-43AA8F4AB173}">
-  <dimension ref="A1:D26"/>
+  <dimension ref="A1:D27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -530,7 +557,7 @@
     <col min="1" max="1" width="102" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19" style="1" customWidth="1"/>
     <col min="3" max="3" width="22" style="1" customWidth="1"/>
-    <col min="4" max="4" width="26.85546875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="36.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
@@ -645,6 +672,12 @@
       <c r="B11" s="1" t="s">
         <v>13</v>
       </c>
+      <c r="C11" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D11" s="4">
+        <v>45441.991666666669</v>
+      </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
@@ -680,95 +713,109 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B17" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="C17" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D16" s="4">
+      <c r="D17" s="4">
         <v>45438.063194444447</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A17" s="1" t="s">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="B18" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A18" s="1" t="s">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" s="1" t="s">
         <v>10</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A19" s="1" t="s">
-        <v>25</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C21" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25" s="1" t="s">
         <v>28</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A25" s="1" t="s">
-        <v>34</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B26" s="1" t="s">
+      <c r="B27" s="1" t="s">
         <v>29</v>
       </c>
     </row>

</xml_diff>

<commit_message>
clean up the fgd file
</commit_message>
<xml_diff>
--- a/docs/version_scheduling/0.0.10.xlsx
+++ b/docs/version_scheduling/0.0.10.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mario\Zombono\docs\version_scheduling\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A67E4F1B-9DB9-436D-A693-6CAFB21BFE49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86F8F95D-640C-4D5E-B432-BB21BEBD1A42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{D1946CF8-FB30-4F75-8FAB-4791887877CB}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="40">
   <si>
     <t>Zombono v0.0.10</t>
   </si>
@@ -163,6 +163,9 @@
   </si>
   <si>
     <t>Fix: Game connects to server during intro on Playtest builds</t>
+  </si>
+  <si>
+    <t>Victory and defeat jingles</t>
   </si>
 </sst>
 </file>
@@ -546,10 +549,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A989902-944C-43B3-895E-43AA8F4AB173}">
-  <dimension ref="A1:D27"/>
+  <dimension ref="A1:D28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -797,15 +800,15 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>28</v>
+        <v>39</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>29</v>
@@ -813,9 +816,17 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A28" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B27" s="1" t="s">
+      <c r="B28" s="1" t="s">
         <v>29</v>
       </c>
     </row>

</xml_diff>

<commit_message>
color4_t refactor, timeui fix
</commit_message>
<xml_diff>
--- a/docs/version_scheduling/0.0.10.xlsx
+++ b/docs/version_scheduling/0.0.10.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mario\Zombono\docs\version_scheduling\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D4D43A2-A526-4F3D-B4AA-2F4D9B8B969E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{177F4F0A-AD65-4E38-B4A8-7C652B9F44AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{D1946CF8-FB30-4F75-8FAB-4791887877CB}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="43">
   <si>
     <t>Zombono v0.0.10</t>
   </si>
@@ -172,6 +172,30 @@
   </si>
   <si>
     <t>Add map and fps meter to cl_showinfo</t>
+  </si>
+  <si>
+    <r>
+      <t>02/06/2024 (</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>REQUIRES POLISHING</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>)</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -558,7 +582,7 @@
   <dimension ref="A1:D28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -685,6 +709,9 @@
       <c r="B10" s="1" t="s">
         <v>13</v>
       </c>
+      <c r="C10" s="3" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
@@ -804,12 +831,18 @@
         <v>36</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>30</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>11</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
@@ -844,12 +877,18 @@
         <v>28</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>33</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>28</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Fixed mouse being snapped to (0,0) in the intro
</commit_message>
<xml_diff>
--- a/docs/version_scheduling/0.0.10.xlsx
+++ b/docs/version_scheduling/0.0.10.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mario\Zombono\docs\version_scheduling\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50448AA8-FEC6-498E-AF60-83BFF08160C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCB9F4FB-371A-4FDD-B291-063A42AB0239}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{D1946CF8-FB30-4F75-8FAB-4791887877CB}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="45">
   <si>
     <t>Zombono v0.0.10</t>
   </si>
@@ -199,6 +199,30 @@
   </si>
   <si>
     <t>Yes (but it sucks)</t>
+  </si>
+  <si>
+    <r>
+      <t>05/06/2024 (</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>REQUIRES POLISHING</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>)</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -585,7 +609,7 @@
   <dimension ref="A1:D28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="A1:XFD1048576"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -746,6 +770,9 @@
       <c r="B12" s="1" t="s">
         <v>13</v>
       </c>
+      <c r="C12" s="3" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
@@ -871,12 +898,18 @@
         <v>11</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>32</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>11</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
make the fucker compile
</commit_message>
<xml_diff>
--- a/docs/version_scheduling/0.0.10.xlsx
+++ b/docs/version_scheduling/0.0.10.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mario\Zombono\docs\version_scheduling\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCB9F4FB-371A-4FDD-B291-063A42AB0239}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{503E5F54-E8D9-48FC-B5E5-126C001BED99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{D1946CF8-FB30-4F75-8FAB-4791887877CB}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="46">
   <si>
     <t>Zombono v0.0.10</t>
   </si>
@@ -223,6 +223,9 @@
       </rPr>
       <t>)</t>
     </r>
+  </si>
+  <si>
+    <t>Deferred to 0.0.11</t>
   </si>
 </sst>
 </file>
@@ -256,7 +259,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -266,6 +269,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -282,7 +291,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -292,6 +301,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -609,7 +619,7 @@
   <dimension ref="A1:D28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -692,6 +702,9 @@
       <c r="B6" s="1" t="s">
         <v>13</v>
       </c>
+      <c r="C6" s="7" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
@@ -795,6 +808,9 @@
       <c r="B14" s="1" t="s">
         <v>13</v>
       </c>
+      <c r="C14" s="7" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
@@ -817,6 +833,9 @@
       <c r="B16" s="1" t="s">
         <v>13</v>
       </c>
+      <c r="C16" s="7" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
@@ -839,6 +858,9 @@
       <c r="B18" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="C18" s="7" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
@@ -847,6 +869,9 @@
       <c r="B19" s="1" t="s">
         <v>11</v>
       </c>
+      <c r="C19" s="7" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
@@ -897,6 +922,9 @@
       <c r="B23" s="1" t="s">
         <v>11</v>
       </c>
+      <c r="C23" s="7" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="24" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
@@ -919,6 +947,12 @@
       <c r="B25" s="1" t="s">
         <v>11</v>
       </c>
+      <c r="C25" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D25" s="4">
+        <v>45451.746527777781</v>
+      </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
@@ -927,6 +961,9 @@
       <c r="B26" s="1" t="s">
         <v>28</v>
       </c>
+      <c r="C26" s="3" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="27" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
@@ -948,6 +985,9 @@
       </c>
       <c r="B28" s="1" t="s">
         <v>28</v>
+      </c>
+      <c r="C28" s="7" t="s">
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>